<commit_message>
Exel Tabelle Planeten Werte
Alle Werte eingetragen
</commit_message>
<xml_diff>
--- a/data/Planeten Werte.xlsx
+++ b/data/Planeten Werte.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Sonne</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Radius  (in m)</t>
   </si>
   <si>
-    <t>Abstand zur Sonne (in m)</t>
-  </si>
-  <si>
     <t>1.989 e33</t>
   </si>
   <si>
@@ -74,37 +71,172 @@
     <t>695,508 e3</t>
   </si>
   <si>
-    <t>2,439.7 e3</t>
-  </si>
-  <si>
-    <t>57,909,227 e3</t>
-  </si>
-  <si>
-    <t>108,209,475 e3</t>
-  </si>
-  <si>
     <t>4.8673 e27</t>
   </si>
   <si>
-    <t>6,051.8 e3</t>
-  </si>
-  <si>
     <t>Mond</t>
   </si>
   <si>
-    <t>6,371.00 e3</t>
-  </si>
-  <si>
-    <t>149,598,262 e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.9722 e27</t>
+    <t>Abstand zur Erde (in m)</t>
+  </si>
+  <si>
+    <t>1737.5 e3</t>
+  </si>
+  <si>
+    <t>7.3477 e25</t>
+  </si>
+  <si>
+    <t>5.9722 e27</t>
+  </si>
+  <si>
+    <t>Equatorial Inclination</t>
+  </si>
+  <si>
+    <t>23.4393</t>
+  </si>
+  <si>
+    <t>2439.7 e3</t>
+  </si>
+  <si>
+    <t>6051.8 e3</t>
+  </si>
+  <si>
+    <t>57909227 e3</t>
+  </si>
+  <si>
+    <t>108209475 e3</t>
+  </si>
+  <si>
+    <t>149598262 e3</t>
+  </si>
+  <si>
+    <t>227943824 e3</t>
+  </si>
+  <si>
+    <t>6.4169 e26</t>
+  </si>
+  <si>
+    <t>3389.5 e3</t>
+  </si>
+  <si>
+    <t>6371.00 e3</t>
+  </si>
+  <si>
+    <t>384400 e3</t>
+  </si>
+  <si>
+    <t>778340821 e3</t>
+  </si>
+  <si>
+    <t>69911 e3</t>
+  </si>
+  <si>
+    <t>5.6832 e29</t>
+  </si>
+  <si>
+    <t>1426666422 e3</t>
+  </si>
+  <si>
+    <t>2870658186 e3</t>
+  </si>
+  <si>
+    <t>8.6810 e28</t>
+  </si>
+  <si>
+    <t>4498396441 e3</t>
+  </si>
+  <si>
+    <t>24622 e3</t>
+  </si>
+  <si>
+    <t>25362 e3</t>
+  </si>
+  <si>
+    <t>58232 e3</t>
+  </si>
+  <si>
+    <t>1.0241 e29</t>
+  </si>
+  <si>
+    <t>1.8981 e30</t>
+  </si>
+  <si>
+    <t>Mittlerer Abstand zur Sonne (in m)</t>
+  </si>
+  <si>
+    <t>Aphel</t>
+  </si>
+  <si>
+    <t>Perihel</t>
+  </si>
+  <si>
+    <t>70 e9</t>
+  </si>
+  <si>
+    <t>46 e9</t>
+  </si>
+  <si>
+    <t>107477 e6</t>
+  </si>
+  <si>
+    <t>108939  e6</t>
+  </si>
+  <si>
+    <t>147095 e6</t>
+  </si>
+  <si>
+    <t>151930 e6</t>
+  </si>
+  <si>
+    <t>206.7 e9</t>
+  </si>
+  <si>
+    <t>249.2 e9</t>
+  </si>
+  <si>
+    <t>778299 e6</t>
+  </si>
+  <si>
+    <t>740550 e6</t>
+  </si>
+  <si>
+    <t>1353.6 e9</t>
+  </si>
+  <si>
+    <t>1513325783 e3</t>
+  </si>
+  <si>
+    <t>2735118.1 e6</t>
+  </si>
+  <si>
+    <t>3006224.7 e6</t>
+  </si>
+  <si>
+    <t>4.459 e12</t>
+  </si>
+  <si>
+    <t>4.537 e12</t>
+  </si>
+  <si>
+    <t>http://www.universetoday.com/21581/neptune/</t>
+  </si>
+  <si>
+    <t>Quelle: http://solarsystem.nasa.gov/planets/mars/facts</t>
+  </si>
+  <si>
+    <t>363300 e3</t>
+  </si>
+  <si>
+    <t>405500 e3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -141,9 +273,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -424,114 +571,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="178" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>